<commit_message>
bug fix: check ru symbols in uk
</commit_message>
<xml_diff>
--- a/finalreport/tests/files/fr/file1.xlsx
+++ b/finalreport/tests/files/fr/file1.xlsx
@@ -8,12 +8,12 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Лист2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Лист3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Лист1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Лист2" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Лист3" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
     <definedName function="false" hidden="false" name="num" vbProcedure="false">[1]ОТЧЕТ_21!$C$1:$D$1048576</definedName>
@@ -192,8 +192,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -292,6 +296,112 @@
 </externalLink>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -303,33 +413,33 @@
       <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
+      <c r="A1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -448,7 +558,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -471,7 +581,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>